<commit_message>
changed protocol for publication date field
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/region/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u050158/django/region/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A4C88F-891C-8744-88A6-865C5AD4C206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C8C728-AF19-2F43-9265-F3B3A6F15328}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" tabRatio="921" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" tabRatio="921" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminary" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Periodical" sheetId="12" r:id="rId8"/>
     <sheet name="Location" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -533,9 +533,6 @@
     <t>If a text is a review, you can add a relation to the publication reviewed. Select the publication from the drop-down menu. If not included, add it by clicking on the + symbol.</t>
   </si>
   <si>
-    <t>Enter the publication date -- year for books and specific month/day for periodicals (e.g. 12 March 1867, or February 1902).</t>
-  </si>
-  <si>
     <t>Here you can add relations to illustrations in the publication. Select the illustration from the drop-down menu. If it's not included, add by clicking on the + symbol.</t>
   </si>
   <si>
@@ -576,6 +573,9 @@
   </si>
   <si>
     <t>Select one ore more locations that contain the current location e.g. if the current location is Madrid you could select Spain</t>
+  </si>
+  <si>
+    <t>Enter the publication date -- year for books and specific month/day for periodicals (e.g.  March 12, 1867 or February 1902).</t>
   </si>
 </sst>
 </file>
@@ -1325,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816CFF2F-B803-4935-AE80-6720B813B8AC}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1385,7 +1385,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1495,7 +1495,7 @@
         <v>34</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1506,7 +1506,7 @@
         <v>35</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1517,7 +1517,7 @@
         <v>36</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1588,7 +1588,7 @@
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1789,7 +1789,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1800,7 +1800,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1822,7 +1822,7 @@
         <v>42</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1844,7 +1844,7 @@
         <v>44</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -2154,7 +2154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -2201,10 +2201,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -2212,10 +2212,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2256,10 +2256,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>